<commit_message>
Menu & Inv Work
</commit_message>
<xml_diff>
--- a/Documents/Agile Documents/Burndown Charts/Burndown - Sprint 3.xlsx
+++ b/Documents/Agile Documents/Burndown Charts/Burndown - Sprint 3.xlsx
@@ -432,19 +432,19 @@
                   <c:v>36.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>36.5</c:v>
+                  <c:v>33.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>36.5</c:v>
+                  <c:v>33.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>36.5</c:v>
+                  <c:v>33.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>36.5</c:v>
+                  <c:v>33.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>36.5</c:v>
+                  <c:v>33.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1511,7 +1511,7 @@
   <dimension ref="A2:J38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1555,23 +1555,23 @@
       </c>
       <c r="D3" s="2">
         <f>$C3-SUM(C7:C38)</f>
-        <v>36.5</v>
+        <v>33.5</v>
       </c>
       <c r="E3" s="2">
         <f>$C3-SUM(C7:D38)</f>
-        <v>36.5</v>
+        <v>33.5</v>
       </c>
       <c r="F3" s="2">
         <f>$C3-SUM(C7:E38)</f>
-        <v>36.5</v>
+        <v>33.5</v>
       </c>
       <c r="G3" s="2">
         <f>$C3-SUM(C7:F38)</f>
-        <v>36.5</v>
+        <v>33.5</v>
       </c>
       <c r="H3" s="2">
         <f>$C3-SUM(C7:G38)</f>
-        <v>36.5</v>
+        <v>33.5</v>
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
@@ -1915,7 +1915,7 @@
         <v>3</v>
       </c>
       <c r="C18" s="8">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D18" s="8">
         <v>0</v>

</xml_diff>

<commit_message>
Sprint 3 Stuff & Meeting Recording
</commit_message>
<xml_diff>
--- a/Documents/Agile Documents/Burndown Charts/Burndown - Sprint 3.xlsx
+++ b/Documents/Agile Documents/Burndown Charts/Burndown - Sprint 3.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2cartj31\Desktop\SWEG-MT-Project-PT2\Documents\Agile Documents\Burndown Charts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\J\Desktop\SWEG-MT-Project-PT2\Documents\Agile Documents\Burndown Charts\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F25EA08A-14B7-4E24-95F6-55698E08B33B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="10110"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="10110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Task</t>
   </si>
@@ -96,11 +97,17 @@
   <si>
     <t>Main menu scene</t>
   </si>
+  <si>
+    <t>Gamepad Input</t>
+  </si>
+  <si>
+    <t>Fix Dialogue</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -292,7 +299,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -365,19 +371,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>36.5</c:v>
+                  <c:v>45.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>29.2</c:v>
+                  <c:v>36.4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>21.9</c:v>
+                  <c:v>27.299999999999997</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>14.599999999999998</c:v>
+                  <c:v>18.199999999999996</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.299999999999998</c:v>
+                  <c:v>9.0999999999999961</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -429,22 +435,22 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>36.5</c:v>
+                  <c:v>45.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>33.5</c:v>
+                  <c:v>42.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>33.5</c:v>
+                  <c:v>42.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>33.5</c:v>
+                  <c:v>42.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>33.5</c:v>
+                  <c:v>42.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>33.5</c:v>
+                  <c:v>42.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -585,7 +591,6 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -593,6 +598,7 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1507,11 +1513,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:J38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1551,27 +1557,27 @@
       </c>
       <c r="C3" s="2">
         <f>SUM(B7:B38)</f>
-        <v>36.5</v>
+        <v>45.5</v>
       </c>
       <c r="D3" s="2">
         <f>$C3-SUM(C7:C38)</f>
-        <v>33.5</v>
+        <v>42.5</v>
       </c>
       <c r="E3" s="2">
         <f>$C3-SUM(C7:D38)</f>
-        <v>33.5</v>
+        <v>42.5</v>
       </c>
       <c r="F3" s="2">
         <f>$C3-SUM(C7:E38)</f>
-        <v>33.5</v>
+        <v>42.5</v>
       </c>
       <c r="G3" s="2">
         <f>$C3-SUM(C7:F38)</f>
-        <v>33.5</v>
+        <v>42.5</v>
       </c>
       <c r="H3" s="2">
         <f>$C3-SUM(C7:G38)</f>
-        <v>33.5</v>
+        <v>42.5</v>
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
@@ -1582,23 +1588,23 @@
       </c>
       <c r="C4" s="9">
         <f>C3</f>
-        <v>36.5</v>
+        <v>45.5</v>
       </c>
       <c r="D4" s="9">
         <f>C4-$C4/5</f>
-        <v>29.2</v>
+        <v>36.4</v>
       </c>
       <c r="E4" s="9">
         <f>D4-$C4/5</f>
-        <v>21.9</v>
+        <v>27.299999999999997</v>
       </c>
       <c r="F4" s="9">
         <f>E4-$C4/5</f>
-        <v>14.599999999999998</v>
+        <v>18.199999999999996</v>
       </c>
       <c r="G4" s="9">
         <f>F4-$C4/5</f>
-        <v>7.299999999999998</v>
+        <v>9.0999999999999961</v>
       </c>
       <c r="H4" s="9">
         <f>G4-$C4/5</f>
@@ -1933,9 +1939,11 @@
       <c r="I18" s="8"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="7"/>
+      <c r="A19" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="B19" s="8">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C19" s="8">
         <v>0</v>
@@ -1956,9 +1964,11 @@
       <c r="I19" s="8"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="7"/>
+      <c r="A20" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="B20" s="8">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C20" s="8">
         <v>0</v>

</xml_diff>

<commit_message>
Meeting Stuff & RAS Hotfix
</commit_message>
<xml_diff>
--- a/Documents/Agile Documents/Burndown Charts/Burndown - Sprint 3.xlsx
+++ b/Documents/Agile Documents/Burndown Charts/Burndown - Sprint 3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\J\Desktop\SWEG-MT-Project-PT2\Documents\Agile Documents\Burndown Charts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD5A85C1-7F81-4DD4-B876-65AD34DDF057}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08490587-1E1B-4E20-8A90-97BC64AAA769}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="10110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -447,10 +447,10 @@
                   <c:v>37.6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>37.6</c:v>
+                  <c:v>32.6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>37.6</c:v>
+                  <c:v>32.6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1516,7 +1516,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:J38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1571,11 +1573,11 @@
       </c>
       <c r="G3" s="2">
         <f>$C3-SUM(C7:F38)</f>
-        <v>37.6</v>
+        <v>32.6</v>
       </c>
       <c r="H3" s="2">
         <f>$C3-SUM(C7:G38)</f>
-        <v>37.6</v>
+        <v>32.6</v>
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
@@ -1728,7 +1730,7 @@
         <v>2</v>
       </c>
       <c r="F10" s="8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G10" s="8">
         <v>0</v>
@@ -1753,7 +1755,7 @@
         <v>0</v>
       </c>
       <c r="F11" s="8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G11" s="8">
         <v>0</v>
@@ -1953,7 +1955,7 @@
         <v>0</v>
       </c>
       <c r="F19" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G19" s="8">
         <v>0</v>

</xml_diff>

<commit_message>
Meeting & Input Support Stuff
</commit_message>
<xml_diff>
--- a/Documents/Agile Documents/Burndown Charts/Burndown - Sprint 3.xlsx
+++ b/Documents/Agile Documents/Burndown Charts/Burndown - Sprint 3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\J\Desktop\SWEG-MT-Project-PT2\Documents\Agile Documents\Burndown Charts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08490587-1E1B-4E20-8A90-97BC64AAA769}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3647910-C80F-414C-967E-4998CA43355F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="10110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Task</t>
   </si>
@@ -102,6 +102,9 @@
   </si>
   <si>
     <t>Fix Dialogue</t>
+  </si>
+  <si>
+    <t>Other Tasks - added for clarity</t>
   </si>
 </sst>
 </file>
@@ -371,19 +374,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>44.5</c:v>
+                  <c:v>51.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>35.6</c:v>
+                  <c:v>41.2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>26.700000000000003</c:v>
+                  <c:v>30.900000000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>17.800000000000004</c:v>
+                  <c:v>20.6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.9000000000000039</c:v>
+                  <c:v>10.3</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -435,22 +438,22 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>44.5</c:v>
+                  <c:v>51.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>41.5</c:v>
+                  <c:v>48.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>39.799999999999997</c:v>
+                  <c:v>46.8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>37.6</c:v>
+                  <c:v>44.6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>32.6</c:v>
+                  <c:v>39.6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32.6</c:v>
+                  <c:v>30.6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1517,7 +1520,7 @@
   <dimension ref="A2:J38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1557,27 +1560,27 @@
       </c>
       <c r="C3" s="2">
         <f>SUM(B7:B38)</f>
-        <v>44.5</v>
+        <v>51.5</v>
       </c>
       <c r="D3" s="2">
         <f>$C3-SUM(C7:C38)</f>
-        <v>41.5</v>
+        <v>48.5</v>
       </c>
       <c r="E3" s="2">
         <f>$C3-SUM(C7:D38)</f>
-        <v>39.799999999999997</v>
+        <v>46.8</v>
       </c>
       <c r="F3" s="2">
         <f>$C3-SUM(C7:E38)</f>
-        <v>37.6</v>
+        <v>44.6</v>
       </c>
       <c r="G3" s="2">
         <f>$C3-SUM(C7:F38)</f>
-        <v>32.6</v>
+        <v>39.6</v>
       </c>
       <c r="H3" s="2">
         <f>$C3-SUM(C7:G38)</f>
-        <v>32.6</v>
+        <v>30.6</v>
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
@@ -1588,23 +1591,23 @@
       </c>
       <c r="C4" s="9">
         <f>C3</f>
-        <v>44.5</v>
+        <v>51.5</v>
       </c>
       <c r="D4" s="9">
         <f>C4-$C4/5</f>
-        <v>35.6</v>
+        <v>41.2</v>
       </c>
       <c r="E4" s="9">
         <f>D4-$C4/5</f>
-        <v>26.700000000000003</v>
+        <v>30.900000000000002</v>
       </c>
       <c r="F4" s="9">
         <f>E4-$C4/5</f>
-        <v>17.800000000000004</v>
+        <v>20.6</v>
       </c>
       <c r="G4" s="9">
         <f>F4-$C4/5</f>
-        <v>8.9000000000000039</v>
+        <v>10.3</v>
       </c>
       <c r="H4" s="9">
         <f>G4-$C4/5</f>
@@ -1783,7 +1786,7 @@
         <v>0</v>
       </c>
       <c r="G12" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12" s="8"/>
       <c r="I12" s="8"/>
@@ -1958,7 +1961,7 @@
         <v>1</v>
       </c>
       <c r="G19" s="8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H19" s="8"/>
       <c r="I19" s="8"/>
@@ -1989,9 +1992,11 @@
       <c r="I20" s="8"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
+      <c r="A21" s="7" t="s">
+        <v>24</v>
+      </c>
       <c r="B21" s="8">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="C21" s="8">
         <v>0</v>
@@ -2006,7 +2011,7 @@
         <v>0</v>
       </c>
       <c r="G21" s="8">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H21" s="8"/>
       <c r="I21" s="8"/>

</xml_diff>